<commit_message>
Refine enemy type presets and simplify logging controls
</commit_message>
<xml_diff>
--- a/_docs/EnemyImbuePresets_MenuMock.xlsx
+++ b/_docs/EnemyImbuePresets_MenuMock.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Preset Impact" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Menu Layout'!$A$1:$H$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Menu Layout'!$A$1:$H$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Preset Impact'!$A$1:$G$87</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -516,7 +516,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H101"/>
+  <dimension ref="A1:H100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4449,27 +4449,27 @@
       </c>
       <c r="B94" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C94" s="2" t="inlineStr">
         <is>
-          <t>Log Level</t>
+          <t>Basic Logs</t>
         </is>
       </c>
       <c r="D94" s="2" t="inlineStr">
         <is>
-          <t>Dropdown</t>
+          <t>Toggle</t>
         </is>
       </c>
       <c r="E94" s="2" t="inlineStr">
         <is>
-          <t>Off | Basic | Diagnostics | Verbose</t>
+          <t>On/Off</t>
         </is>
       </c>
       <c r="F94" s="2" t="inlineStr">
         <is>
-          <t>Basic</t>
+          <t>On</t>
         </is>
       </c>
       <c r="G94" s="2" t="inlineStr">
@@ -4479,7 +4479,7 @@
       </c>
       <c r="H94" s="2" t="inlineStr">
         <is>
-          <t>Logging detail</t>
+          <t>General informational logging</t>
         </is>
       </c>
     </row>
@@ -4491,27 +4491,27 @@
       </c>
       <c r="B95" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C95" s="2" t="inlineStr">
         <is>
-          <t>Imbue Update Interval</t>
+          <t>Diagnostics Logs</t>
         </is>
       </c>
       <c r="D95" s="2" t="inlineStr">
         <is>
-          <t>Dropdown</t>
+          <t>Toggle</t>
         </is>
       </c>
       <c r="E95" s="2" t="inlineStr">
         <is>
-          <t>0.05s..1.00s</t>
+          <t>On/Off</t>
         </is>
       </c>
       <c r="F95" s="2" t="inlineStr">
         <is>
-          <t>0.25s</t>
+          <t>Off</t>
         </is>
       </c>
       <c r="G95" s="2" t="inlineStr">
@@ -4521,7 +4521,7 @@
       </c>
       <c r="H95" s="2" t="inlineStr">
         <is>
-          <t>Performance/response tradeoff</t>
+          <t>Deeper troubleshooting logs</t>
         </is>
       </c>
     </row>
@@ -4533,27 +4533,27 @@
       </c>
       <c r="B96" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C96" s="2" t="inlineStr">
         <is>
-          <t>Enemy Rescan Interval</t>
+          <t>Verbose Logs</t>
         </is>
       </c>
       <c r="D96" s="2" t="inlineStr">
         <is>
-          <t>Dropdown</t>
+          <t>Toggle</t>
         </is>
       </c>
       <c r="E96" s="2" t="inlineStr">
         <is>
-          <t>0.50s..5.00s</t>
+          <t>On/Off</t>
         </is>
       </c>
       <c r="F96" s="2" t="inlineStr">
         <is>
-          <t>2.00s</t>
+          <t>Off</t>
         </is>
       </c>
       <c r="G96" s="2" t="inlineStr">
@@ -4563,7 +4563,7 @@
       </c>
       <c r="H96" s="2" t="inlineStr">
         <is>
-          <t>Tracking refresh interval</t>
+          <t>High-volume per-creature logs</t>
         </is>
       </c>
     </row>
@@ -4575,27 +4575,27 @@
       </c>
       <c r="B97" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C97" s="2" t="inlineStr">
         <is>
-          <t>Dump Factions</t>
+          <t>Session Diagnostics</t>
         </is>
       </c>
       <c r="D97" s="2" t="inlineStr">
         <is>
-          <t>Button</t>
+          <t>Toggle</t>
         </is>
       </c>
       <c r="E97" s="2" t="inlineStr">
         <is>
-          <t>False/True</t>
+          <t>On/Off</t>
         </is>
       </c>
       <c r="F97" s="2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>Off</t>
         </is>
       </c>
       <c r="G97" s="2" t="inlineStr">
@@ -4605,7 +4605,7 @@
       </c>
       <c r="H97" s="2" t="inlineStr">
         <is>
-          <t>One-shot debug action</t>
+          <t>Structured session summary logs</t>
         </is>
       </c>
     </row>
@@ -4617,27 +4617,27 @@
       </c>
       <c r="B98" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C98" s="2" t="inlineStr">
         <is>
-          <t>Dump Wave-Faction Map</t>
+          <t>Imbue Update Interval</t>
         </is>
       </c>
       <c r="D98" s="2" t="inlineStr">
         <is>
-          <t>Button</t>
+          <t>Dropdown</t>
         </is>
       </c>
       <c r="E98" s="2" t="inlineStr">
         <is>
-          <t>False/True</t>
+          <t>0.05s..1.00s</t>
         </is>
       </c>
       <c r="F98" s="2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>0.25s</t>
         </is>
       </c>
       <c r="G98" s="2" t="inlineStr">
@@ -4647,7 +4647,7 @@
       </c>
       <c r="H98" s="2" t="inlineStr">
         <is>
-          <t>One-shot debug action</t>
+          <t>Performance/response tradeoff</t>
         </is>
       </c>
     </row>
@@ -4659,27 +4659,27 @@
       </c>
       <c r="B99" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C99" s="2" t="inlineStr">
         <is>
-          <t>Dump State</t>
+          <t>Enemy Rescan Interval</t>
         </is>
       </c>
       <c r="D99" s="2" t="inlineStr">
         <is>
-          <t>Button</t>
+          <t>Dropdown</t>
         </is>
       </c>
       <c r="E99" s="2" t="inlineStr">
         <is>
-          <t>False/True</t>
+          <t>0.50s..5.00s</t>
         </is>
       </c>
       <c r="F99" s="2" t="inlineStr">
         <is>
-          <t>False</t>
+          <t>2.00s</t>
         </is>
       </c>
       <c r="G99" s="2" t="inlineStr">
@@ -4689,7 +4689,7 @@
       </c>
       <c r="H99" s="2" t="inlineStr">
         <is>
-          <t>One-shot debug action</t>
+          <t>Tracking refresh interval</t>
         </is>
       </c>
     </row>
@@ -4701,12 +4701,12 @@
       </c>
       <c r="B100" s="2" t="inlineStr">
         <is>
-          <t>Diagnostics</t>
+          <t>Advanced</t>
         </is>
       </c>
       <c r="C100" s="2" t="inlineStr">
         <is>
-          <t>Dump Enemy Type Detection</t>
+          <t>Force Reapply</t>
         </is>
       </c>
       <c r="D100" s="2" t="inlineStr">
@@ -4731,54 +4731,12 @@
       </c>
       <c r="H100" s="2" t="inlineStr">
         <is>
-          <t>One-shot debug action</t>
-        </is>
-      </c>
-    </row>
-    <row r="101">
-      <c r="A101" s="2" t="inlineStr">
-        <is>
-          <t>1006</t>
-        </is>
-      </c>
-      <c r="B101" s="2" t="inlineStr">
-        <is>
-          <t>Diagnostics</t>
-        </is>
-      </c>
-      <c r="C101" s="2" t="inlineStr">
-        <is>
-          <t>Force Reapply</t>
-        </is>
-      </c>
-      <c r="D101" s="2" t="inlineStr">
-        <is>
-          <t>Button</t>
-        </is>
-      </c>
-      <c r="E101" s="2" t="inlineStr">
-        <is>
-          <t>False/True</t>
-        </is>
-      </c>
-      <c r="F101" s="2" t="inlineStr">
-        <is>
-          <t>False</t>
-        </is>
-      </c>
-      <c r="G101" s="2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="H101" s="2" t="inlineStr">
-        <is>
-          <t>One-shot debug action</t>
+          <t>One-shot reapply action</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H101"/>
+  <autoFilter ref="A1:H100"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>